<commit_message>
replace pdf to EN version. update steering and brake wattage estimation
</commit_message>
<xml_diff>
--- a/Power/electrical_parts_list.xlsx
+++ b/Power/electrical_parts_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevSpace\Projects\FormulaAV2020\Hardware_Algo\Power\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7904AACA-634C-49F4-98F0-07239D348F24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED3920B-BBF0-4959-BC6B-B0208CD17850}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{FD6B09E7-CAE9-46B4-9648-433F28AAFF9C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="69">
   <si>
     <t>max current</t>
   </si>
@@ -216,6 +216,33 @@
   </si>
   <si>
     <t>wattage is the worst case for optional lidar. Current lidar powered by the autonoumus pc</t>
+  </si>
+  <si>
+    <t>controller voltage supply  12-50V. motor input 0-50V. Wattage is not include motor wattage</t>
+  </si>
+  <si>
+    <t>anti rool servos (4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anti rool servos controller (4) </t>
+  </si>
+  <si>
+    <t>estimate.</t>
+  </si>
+  <si>
+    <t>wing controller</t>
+  </si>
+  <si>
+    <t>wing motor</t>
+  </si>
+  <si>
+    <t>colling pump</t>
+  </si>
+  <si>
+    <t>cooling fan</t>
+  </si>
+  <si>
+    <t>SPAL VA32-A101-62A 12V 3.4A-MAX</t>
   </si>
 </sst>
 </file>
@@ -619,15 +646,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99AB1913-3ACA-4A36-ADF0-5064DFF99C18}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" style="5" customWidth="1"/>
     <col min="2" max="3" width="33.140625" style="6" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" style="6" customWidth="1"/>
     <col min="5" max="5" width="21.140625" style="6" customWidth="1"/>
@@ -713,16 +740,18 @@
       <c r="G4" s="9"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9" t="s">
-        <v>35</v>
+      <c r="C5" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="9">
+        <v>24</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -739,16 +768,22 @@
         <v>31</v>
       </c>
       <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="F6" s="9">
+        <v>200</v>
+      </c>
       <c r="G6" s="9"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
+      <c r="B7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="D7" s="9" t="s">
         <v>35</v>
       </c>
@@ -762,12 +797,16 @@
         <v>33</v>
       </c>
       <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="D8" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="F8" s="9">
+        <v>100</v>
+      </c>
       <c r="G8" s="9"/>
       <c r="H8" s="7"/>
     </row>
@@ -861,87 +900,126 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4" t="s">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F24" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G24" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="35" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4" t="s">
+      <c r="C35" s="4"/>
+      <c r="D35" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E35" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F35" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G35" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D36" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="G36" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update devices wattage estimation
</commit_message>
<xml_diff>
--- a/Power/electrical_parts_list.xlsx
+++ b/Power/electrical_parts_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevSpace\Projects\FormulaAV2020\Hardware_Algo\Power\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED3920B-BBF0-4959-BC6B-B0208CD17850}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E52DD4A-40A4-4C61-83F1-E58F9CBECE2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{FD6B09E7-CAE9-46B4-9648-433F28AAFF9C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="77">
   <si>
     <t>max current</t>
   </si>
@@ -116,42 +116,24 @@
     <t>EBS</t>
   </si>
   <si>
-    <t>5V</t>
-  </si>
-  <si>
     <t>custom: pc- teensy3.2, logic-custom</t>
   </si>
   <si>
-    <t>(build in)</t>
-  </si>
-  <si>
     <t>EBS sensors</t>
   </si>
   <si>
     <t>DC-DC convertor 24,5</t>
   </si>
   <si>
-    <t>from steering contoller</t>
-  </si>
-  <si>
     <t>brake controller</t>
   </si>
   <si>
     <t>brake motor</t>
   </si>
   <si>
-    <t>from brake controller</t>
-  </si>
-  <si>
-    <t>24V</t>
-  </si>
-  <si>
     <t>Faulhaber MC-5010S</t>
   </si>
   <si>
-    <t>Teensy 3.2</t>
-  </si>
-  <si>
     <t>brake?</t>
   </si>
   <si>
@@ -164,9 +146,6 @@
     <t>7-60V</t>
   </si>
   <si>
-    <t>9W max</t>
-  </si>
-  <si>
     <t>fuse (DE7.3.3)</t>
   </si>
   <si>
@@ -212,24 +191,15 @@
     <t>current peak 130A/200us</t>
   </si>
   <si>
-    <t>power by the autonomuos pc</t>
-  </si>
-  <si>
     <t>wattage is the worst case for optional lidar. Current lidar powered by the autonoumus pc</t>
   </si>
   <si>
-    <t>controller voltage supply  12-50V. motor input 0-50V. Wattage is not include motor wattage</t>
-  </si>
-  <si>
     <t>anti rool servos (4)</t>
   </si>
   <si>
     <t xml:space="preserve">anti rool servos controller (4) </t>
   </si>
   <si>
-    <t>estimate.</t>
-  </si>
-  <si>
     <t>wing controller</t>
   </si>
   <si>
@@ -243,6 +213,60 @@
   </si>
   <si>
     <t>SPAL VA32-A101-62A 12V 3.4A-MAX</t>
+  </si>
+  <si>
+    <t>power by the autonomuos pc. Wattage include in pc power</t>
+  </si>
+  <si>
+    <t>Teensy 3.2+screen/motec D153</t>
+  </si>
+  <si>
+    <t>estimate by motec D153 typical power</t>
+  </si>
+  <si>
+    <t>ASSI(3) + Break light + buzzer</t>
+  </si>
+  <si>
+    <t>estimate by 3 watt each</t>
+  </si>
+  <si>
+    <t>from rule book: 12-24V 0.26A@12V</t>
+  </si>
+  <si>
+    <t>controller voltage supply  12-50V, CANopen version current 0.06A@24V. motor input 0-50V. Wattage is not include motor wattage</t>
+  </si>
+  <si>
+    <t>estimate by RES</t>
+  </si>
+  <si>
+    <t>5-36V, 6mW max</t>
+  </si>
+  <si>
+    <t>estimate by assuming it need the same power as brake</t>
+  </si>
+  <si>
+    <t>estimate by comparation the require Force(N) with brake system</t>
+  </si>
+  <si>
+    <t>estimate as mc5010</t>
+  </si>
+  <si>
+    <t>cant find info. Estimate by some forum</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>estimete</t>
+  </si>
+  <si>
+    <t>SUM 12V</t>
+  </si>
+  <si>
+    <t>SUM 24V</t>
+  </si>
+  <si>
+    <t>estimate. Powered from steering contoller</t>
   </si>
 </sst>
 </file>
@@ -279,15 +303,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -295,11 +325,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -331,6 +370,24 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99AB1913-3ACA-4A36-ADF0-5064DFF99C18}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,16 +728,16 @@
         <v>23</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>2</v>
@@ -688,13 +745,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="D2" s="6">
         <v>12</v>
@@ -706,7 +763,7 @@
         <v>456</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="H2" s="7"/>
     </row>
@@ -716,9 +773,11 @@
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="9"/>
+        <v>51</v>
+      </c>
+      <c r="D3" s="9">
+        <v>12</v>
+      </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9">
         <v>32</v>
@@ -726,13 +785,13 @@
       <c r="G3" s="9"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -740,21 +799,23 @@
       <c r="G4" s="9"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D5" s="9">
         <v>24</v>
       </c>
       <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="F5" s="9">
+        <v>1.44</v>
+      </c>
       <c r="G5" s="9"/>
       <c r="H5" s="7"/>
     </row>
@@ -763,9 +824,11 @@
         <v>18</v>
       </c>
       <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9" t="s">
-        <v>31</v>
+      <c r="C6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="9">
+        <v>24</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9">
@@ -774,34 +837,36 @@
       <c r="G6" s="9"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>35</v>
+        <v>65</v>
+      </c>
+      <c r="D7" s="9">
+        <v>24</v>
       </c>
       <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+      <c r="F7" s="9">
+        <v>1.44</v>
+      </c>
       <c r="G7" s="9"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>34</v>
+        <v>76</v>
+      </c>
+      <c r="D8" s="9">
+        <v>24</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9">
@@ -815,38 +880,54 @@
         <v>16</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9" t="s">
-        <v>26</v>
+        <v>60</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="9">
+        <v>24</v>
       </c>
       <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="F9" s="9">
+        <v>5.32</v>
+      </c>
       <c r="G9" s="9"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
+      <c r="C10" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="9">
+        <v>24</v>
+      </c>
       <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="F10" s="9">
+        <v>15</v>
+      </c>
       <c r="G10" s="9"/>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
+      <c r="C11" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="9">
+        <v>24</v>
+      </c>
       <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
+      <c r="F11" s="9">
+        <v>3.12</v>
+      </c>
       <c r="G11" s="9"/>
       <c r="H11" s="7"/>
     </row>
@@ -855,172 +936,287 @@
         <v>25</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9" t="s">
         <v>26</v>
       </c>
+      <c r="C12" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="9">
+        <v>24</v>
+      </c>
       <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10" t="s">
-        <v>28</v>
-      </c>
+      <c r="F12" s="9">
+        <v>4</v>
+      </c>
+      <c r="G12" s="10"/>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9" t="s">
-        <v>41</v>
+        <v>34</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="6">
+        <v>24</v>
       </c>
       <c r="E13" s="9"/>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="9">
+        <v>9</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>49</v>
+      <c r="C14" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="6">
+        <v>12</v>
+      </c>
+      <c r="E14" s="6">
+        <v>5.5</v>
+      </c>
+      <c r="F14" s="6">
+        <v>66</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="6">
+        <v>24</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0.6</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="6">
+        <v>24</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="6">
+        <v>24</v>
+      </c>
+      <c r="F17" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="6">
+        <v>24</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>65</v>
+        <v>55</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="6">
+        <v>24</v>
+      </c>
+      <c r="F19" s="6">
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>66</v>
+        <v>56</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="D20" s="6">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="F20" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="16">
         <v>12</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="E21" s="16">
+        <v>3.4</v>
+      </c>
+      <c r="F21" s="16">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14">
+        <f>SUM(F2:F21)</f>
+        <v>1307.6000000000001</v>
+      </c>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14">
+        <f>SUMIF(D2:D21,12,F2:F21)</f>
+        <v>594.79999999999995</v>
+      </c>
+      <c r="G23" s="14"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="14">
+        <f>SUMIF(D2:D21,24,F2:F21)</f>
+        <v>712.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4" t="s">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G26" s="4" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4" t="s">
+      <c r="C37" s="4"/>
+      <c r="D37" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E37" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F37" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="G37" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G36" s="6" t="s">
+      <c r="G38" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>30</v>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1075,12 +1271,12 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1115,10 +1311,10 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
@@ -1133,12 +1329,12 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
@@ -1153,7 +1349,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1206,12 +1402,12 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -1246,7 +1442,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
@@ -1261,12 +1457,12 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
@@ -1281,7 +1477,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1334,12 +1530,12 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -1374,7 +1570,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
@@ -1389,12 +1585,12 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
@@ -1409,7 +1605,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update brake actuator details
</commit_message>
<xml_diff>
--- a/Power/electrical_parts_list.xlsx
+++ b/Power/electrical_parts_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevSpace\Projects\FormulaAV2020\Hardware_Algo\Power\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BB2FEA-2514-4170-8895-987FA288C856}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA59F98-1B07-4BCD-8275-D05F2C4904D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{FD6B09E7-CAE9-46B4-9648-433F28AAFF9C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="81">
   <si>
     <t>max current</t>
   </si>
@@ -270,6 +270,17 @@
   </si>
   <si>
     <t>24*4</t>
+  </si>
+  <si>
+    <t>Faulhaber DC-Micromotors
+Series 3890H024CR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Powered from steering contoller. Planetary Gearheads
+Series 38/2 S</t>
+  </si>
+  <si>
+    <t>BOTS</t>
   </si>
 </sst>
 </file>
@@ -370,7 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -429,6 +440,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -747,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99AB1913-3ACA-4A36-ADF0-5064DFF99C18}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,20 +913,22 @@
       <c r="G7" s="9"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9" t="s">
-        <v>76</v>
+      <c r="B8" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>79</v>
       </c>
       <c r="D8" s="9">
         <v>24</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="19">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="7"/>
@@ -1154,7 +1170,7 @@
       <c r="E22" s="14"/>
       <c r="F22" s="14">
         <f>SUM(F2:F21)</f>
-        <v>1307.9200000000003</v>
+        <v>1367.9200000000003</v>
       </c>
       <c r="G22" s="14"/>
     </row>
@@ -1178,7 +1194,7 @@
       </c>
       <c r="F24" s="14">
         <f>SUMIF(D2:D21,24,F2:F21)</f>
-        <v>617.12</v>
+        <v>677.12</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1225,6 +1241,11 @@
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
start to cahnge the table to contain more components
</commit_message>
<xml_diff>
--- a/Power/electrical_parts_list.xlsx
+++ b/Power/electrical_parts_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevSpace\Projects\FormulaAV2020\Hardware_Algo\Power\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BB2FEA-2514-4170-8895-987FA288C856}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0C2FB3-A7FE-42AA-A2A2-94332F4CF490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{FD6B09E7-CAE9-46B4-9648-433F28AAFF9C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="94">
   <si>
     <t>max current</t>
   </si>
@@ -182,9 +182,6 @@
     <t>max wattage (W)</t>
   </si>
   <si>
-    <t>note</t>
-  </si>
-  <si>
     <t>max current (A)</t>
   </si>
   <si>
@@ -270,6 +267,57 @@
   </si>
   <si>
     <t>24*4</t>
+  </si>
+  <si>
+    <t>Datasheet</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>https://github.com/TechnionAVFormula/Hardware_Algo/blob/staging/Power/NVIDIA%20AGX%20Xavier/DRIVE%20AGX%20Developer%20Kit%20Mechanical%20%26%20Installation%20Guide.pdf</t>
+  </si>
+  <si>
+    <t>rear, above the motor and inverter</t>
+  </si>
+  <si>
+    <t>main hoop</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>General Information</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Connectors</t>
+  </si>
+  <si>
+    <t>controllers</t>
+  </si>
+  <si>
+    <t>actuators</t>
+  </si>
+  <si>
+    <t>switches</t>
+  </si>
+  <si>
+    <t>connectors</t>
   </si>
 </sst>
 </file>
@@ -370,7 +418,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -429,6 +477,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -745,527 +799,634 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99AB1913-3ACA-4A36-ADF0-5064DFF99C18}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="5" customWidth="1"/>
-    <col min="2" max="3" width="33.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="6" customWidth="1"/>
-    <col min="7" max="8" width="25.7109375" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="25.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="5" customWidth="1"/>
+    <col min="3" max="5" width="33.140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" style="6" customWidth="1"/>
+    <col min="9" max="10" width="25.7109375" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B1" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+    </row>
+    <row r="2" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="H2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="6">
+        <v>12</v>
+      </c>
+      <c r="G3" s="6">
+        <v>38</v>
+      </c>
+      <c r="H3" s="6">
+        <v>456</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="6">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9">
         <v>12</v>
       </c>
-      <c r="E2" s="6">
-        <v>38</v>
-      </c>
-      <c r="F2" s="6">
-        <v>456</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="9">
-        <v>12</v>
-      </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9">
         <v>32</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="7"/>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="I4" s="9"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="21"/>
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:22" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="21"/>
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="C6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" s="9">
+      <c r="D6" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9">
         <v>24</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9">
+      <c r="G6" s="9"/>
+      <c r="H6" s="9">
         <v>1.44</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="I6" s="9"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:22" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="21"/>
+      <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" s="9">
-        <v>24</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="19">
-        <v>200</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="9">
-        <v>24</v>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9">
+        <v>24</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="19">
+        <v>200</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:22" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="21"/>
+      <c r="B8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9">
+        <v>24</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9">
         <v>1.44</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="I8" s="9"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:22" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="21"/>
+      <c r="B9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="9">
-        <v>24</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="19">
-        <v>100</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="9">
-        <v>24</v>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9">
-        <v>5.32</v>
+        <v>24</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="9"/>
+      <c r="H9" s="19">
+        <v>100</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:22" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="C10" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="9">
-        <v>24</v>
+        <v>59</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G10" s="9"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="9">
-        <v>24</v>
+      <c r="H10" s="9">
+        <v>5.32</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9">
-        <v>3.12</v>
+        <v>24</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="9">
-        <v>24</v>
+      <c r="H11" s="9">
+        <v>15</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9">
-        <v>4</v>
-      </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>34</v>
+        <v>24</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9">
+        <v>3.12</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="6">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9">
+        <v>24</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9">
+        <v>4</v>
+      </c>
+      <c r="I13" s="10"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="21"/>
+      <c r="B14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="6">
+        <v>24</v>
+      </c>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9">
         <v>9</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="I14" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:8" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:22" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="21"/>
+      <c r="B15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="6">
+      <c r="D15" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="6">
         <v>12</v>
       </c>
-      <c r="E14" s="18">
+      <c r="G15" s="18">
         <v>5.5</v>
       </c>
-      <c r="F14" s="18">
+      <c r="H15" s="18">
         <v>66</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="6">
+      <c r="D16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="6">
         <v>24</v>
       </c>
-      <c r="F15" s="6">
+      <c r="H16" s="6">
         <v>0.6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="6">
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="6">
         <v>24</v>
       </c>
-      <c r="F16" s="6">
+      <c r="H17" s="6">
         <f>1.44*4</f>
         <v>5.76</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="12" t="s">
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="6">
+        <v>12</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" s="20">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="21"/>
+      <c r="B19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="6">
+        <v>24</v>
+      </c>
+      <c r="H19" s="6">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="21"/>
+      <c r="B20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="6">
+      <c r="E20" s="12"/>
+      <c r="F20" s="6">
+        <v>24</v>
+      </c>
+      <c r="H20" s="18">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="21"/>
+      <c r="B21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="17"/>
+      <c r="F21" s="6">
+        <v>24</v>
+      </c>
+      <c r="H21" s="18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="21"/>
+      <c r="B22" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16">
         <v>12</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F17" s="20">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="6">
-        <v>24</v>
-      </c>
-      <c r="F18" s="6">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="6">
-        <v>24</v>
-      </c>
-      <c r="F19" s="18">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="6">
-        <v>24</v>
-      </c>
-      <c r="F20" s="18">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="16">
-        <v>12</v>
-      </c>
-      <c r="E21" s="16">
+      <c r="G22" s="16">
         <v>3.4</v>
       </c>
-      <c r="F21" s="16">
+      <c r="H22" s="16">
         <v>40.799999999999997</v>
       </c>
-      <c r="G21" s="16"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14">
-        <f>SUM(F2:F21)</f>
-        <v>1307.9200000000003</v>
-      </c>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" s="14"/>
+      <c r="I22" s="16"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>71</v>
+      </c>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
-      <c r="F23" s="14">
-        <f>SUMIF(D2:D21,12,F2:F21)</f>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14">
+        <f>SUM(H3:H22)</f>
+        <v>1307.9200000000003</v>
+      </c>
+      <c r="I23" s="14"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14">
+        <f>SUMIF(F3:F22,12,H3:H22)</f>
         <v>690.8</v>
       </c>
-      <c r="G23" s="14"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F24" s="14">
-        <f>SUMIF(D2:D21,24,F2:F21)</f>
+      <c r="I24" s="14"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H25" s="14">
+        <f>SUMIF(F3:F22,24,H3:H22)</f>
         <v>617.12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4" t="s">
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="G27" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="I27" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="38" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4" t="s">
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="G38" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="H38" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="I38" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="F39" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="6" t="s">
+      <c r="I39" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="A3:A22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1533,88 +1694,121 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52781356-E028-4A84-92DD-F3EC2AB72D88}">
-  <dimension ref="A1:A33"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1656,5 +1850,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>